<commit_message>
minimal example as far as code goes
</commit_message>
<xml_diff>
--- a/inst/extdata/example_varInfo.xlsx
+++ b/inst/extdata/example_varInfo.xlsx
@@ -683,7 +683,7 @@
         <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -933,7 +933,7 @@
         <v>18</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M9" t="s">
         <v>18</v>
@@ -1083,7 +1083,7 @@
         <v>18</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M12" t="s">
         <v>18</v>
@@ -1133,7 +1133,7 @@
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M13" t="s">
         <v>18</v>
@@ -1183,7 +1183,7 @@
         <v>18</v>
       </c>
       <c r="L14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M14" t="s">
         <v>18</v>
@@ -1233,7 +1233,7 @@
         <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M15" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
fix order in varInfo
</commit_message>
<xml_diff>
--- a/inst/extdata/example_varInfo.xlsx
+++ b/inst/extdata/example_varInfo.xlsx
@@ -614,9 +614,7 @@
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
+      <c r="H2"/>
       <c r="I2" t="s">
         <v>22</v>
       </c>
@@ -667,9 +665,7 @@
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
+      <c r="H3"/>
       <c r="I3" t="s">
         <v>25</v>
       </c>
@@ -720,9 +716,7 @@
       <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
+      <c r="H4"/>
       <c r="I4" t="s">
         <v>27</v>
       </c>
@@ -773,9 +767,7 @@
       <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
+      <c r="H5"/>
       <c r="I5" t="s">
         <v>30</v>
       </c>
@@ -826,9 +818,7 @@
       <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
+      <c r="H6"/>
       <c r="I6" t="s">
         <v>20</v>
       </c>
@@ -879,9 +869,7 @@
       <c r="G7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
+      <c r="H7"/>
       <c r="I7" t="s">
         <v>20</v>
       </c>
@@ -932,9 +920,7 @@
       <c r="G8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
+      <c r="H8"/>
       <c r="I8" t="s">
         <v>20</v>
       </c>
@@ -985,9 +971,7 @@
       <c r="G9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
+      <c r="H9"/>
       <c r="I9" t="s">
         <v>39</v>
       </c>
@@ -1036,9 +1020,7 @@
       <c r="G10" t="s">
         <v>43</v>
       </c>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
+      <c r="H10"/>
       <c r="I10" t="s">
         <v>44</v>
       </c>
@@ -1089,9 +1071,7 @@
       <c r="G11" t="s">
         <v>43</v>
       </c>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
+      <c r="H11"/>
       <c r="I11" t="s">
         <v>20</v>
       </c>
@@ -1142,9 +1122,7 @@
       <c r="G12" t="s">
         <v>43</v>
       </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
+      <c r="H12"/>
       <c r="I12" t="s">
         <v>20</v>
       </c>
@@ -1195,9 +1173,7 @@
       <c r="G13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" t="s">
-        <v>20</v>
-      </c>
+      <c r="H13"/>
       <c r="I13" t="s">
         <v>20</v>
       </c>
@@ -1248,9 +1224,7 @@
       <c r="G14" t="s">
         <v>43</v>
       </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
+      <c r="H14"/>
       <c r="I14" t="s">
         <v>20</v>
       </c>
@@ -1301,9 +1275,7 @@
       <c r="G15" t="s">
         <v>43</v>
       </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
+      <c r="H15"/>
       <c r="I15" t="s">
         <v>20</v>
       </c>
@@ -1352,9 +1324,7 @@
       <c r="G16" t="s">
         <v>43</v>
       </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
+      <c r="H16"/>
       <c r="I16" t="s">
         <v>56</v>
       </c>
@@ -1405,9 +1375,7 @@
       <c r="G17" t="s">
         <v>43</v>
       </c>
-      <c r="H17" t="s">
-        <v>20</v>
-      </c>
+      <c r="H17"/>
       <c r="I17" t="s">
         <v>20</v>
       </c>
@@ -1458,9 +1426,7 @@
       <c r="G18" t="s">
         <v>43</v>
       </c>
-      <c r="H18" t="s">
-        <v>20</v>
-      </c>
+      <c r="H18"/>
       <c r="I18" t="s">
         <v>20</v>
       </c>
@@ -1511,9 +1477,7 @@
       <c r="G19" t="s">
         <v>43</v>
       </c>
-      <c r="H19" t="s">
-        <v>20</v>
-      </c>
+      <c r="H19"/>
       <c r="I19" t="s">
         <v>20</v>
       </c>
@@ -1564,9 +1528,7 @@
       <c r="G20" t="s">
         <v>43</v>
       </c>
-      <c r="H20" t="s">
-        <v>20</v>
-      </c>
+      <c r="H20"/>
       <c r="I20" t="s">
         <v>20</v>
       </c>
@@ -1617,9 +1579,7 @@
       <c r="G21" t="s">
         <v>43</v>
       </c>
-      <c r="H21" t="s">
-        <v>20</v>
-      </c>
+      <c r="H21"/>
       <c r="I21" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
New vignette version + codebook pdf
</commit_message>
<xml_diff>
--- a/inst/extdata/example_varInfo.xlsx
+++ b/inst/extdata/example_varInfo.xlsx
@@ -1,229 +1,239 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bussejoh\Desktop\eatCodebook\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C466F2B2-EDEF-4492-ABCA-3650E36EE266}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
-  <si>
-    <t xml:space="preserve">Var.Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in.DS.und.SH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unterteilung.im.Skalenhandbuch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LabelSH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anmerkung.Var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gliederung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reihenfolge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rekodiert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QuelleSH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instruktionen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hintergrundmodell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HGM.Reihenfolge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HGM.Variable.erstellt.aus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intern.extern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seitenumbruch.im.Inhaltsverzeichnis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schueler-ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDSCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School-ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varMetrisch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metrische Beispielvariable, Kompetenzwert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varOrdinal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ordinale Beispielvariable, Kompetenzstufe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mueller (2019)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varCat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nominale Beispielvariable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skala1_item1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Likert-Skalenindikator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skala1_item2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skala1_item3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skala1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skala: Likert-Skalenwert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_pooled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PVs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plausible Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 1: plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 2: plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 3: plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 4: plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 5: plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvkat_pooled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categorical plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvkat_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 1: Kompetenzstufe des plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvkat_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 2: Kompetenzstufe des plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvkat_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 3: Kompetenzstufe des plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvkat_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPUTATION 4: Kompetenzstufe des plausible value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pvkat_5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="69">
+  <si>
+    <t>Var.Name</t>
+  </si>
+  <si>
+    <t>in.DS.und.SH</t>
+  </si>
+  <si>
+    <t>Unterteilung.im.Skalenhandbuch</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>LabelSH</t>
+  </si>
+  <si>
+    <t>Anmerkung.Var</t>
+  </si>
+  <si>
+    <t>Gliederung</t>
+  </si>
+  <si>
+    <t>Reihenfolge</t>
+  </si>
+  <si>
+    <t>Titel</t>
+  </si>
+  <si>
+    <t>rekodiert</t>
+  </si>
+  <si>
+    <t>QuelleSH</t>
+  </si>
+  <si>
+    <t>Instruktionen</t>
+  </si>
+  <si>
+    <t>Hintergrundmodell</t>
+  </si>
+  <si>
+    <t>HGM.Reihenfolge</t>
+  </si>
+  <si>
+    <t>HGM.Variable.erstellt.aus</t>
+  </si>
+  <si>
+    <t>intern.extern</t>
+  </si>
+  <si>
+    <t>Seitenumbruch.im.Inhaltsverzeichnis</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Schueler-ID</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>IDSCH</t>
+  </si>
+  <si>
+    <t>School-ID</t>
+  </si>
+  <si>
+    <t>varMetrisch</t>
+  </si>
+  <si>
+    <t>metrische Beispielvariable, Kompetenzwert</t>
+  </si>
+  <si>
+    <t>varOrdinal</t>
+  </si>
+  <si>
+    <t>ordinale Beispielvariable, Kompetenzstufe</t>
+  </si>
+  <si>
+    <t>Mueller (2019)</t>
+  </si>
+  <si>
+    <t>varCat</t>
+  </si>
+  <si>
+    <t>nominale Beispielvariable</t>
+  </si>
+  <si>
+    <t>skala1_item1</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Likert-Skalenindikator</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>skala1_item2</t>
+  </si>
+  <si>
+    <t>skala1_item3</t>
+  </si>
+  <si>
+    <t>skala1</t>
+  </si>
+  <si>
+    <t>Skala: Likert-Skalenwert</t>
+  </si>
+  <si>
+    <t>pv_pooled</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>PVs</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Plausible Value</t>
+  </si>
+  <si>
+    <t>pv_1</t>
+  </si>
+  <si>
+    <t>IMPUTATION 1: plausible value</t>
+  </si>
+  <si>
+    <t>pv_2</t>
+  </si>
+  <si>
+    <t>IMPUTATION 2: plausible value</t>
+  </si>
+  <si>
+    <t>pv_3</t>
+  </si>
+  <si>
+    <t>IMPUTATION 3: plausible value</t>
+  </si>
+  <si>
+    <t>pv_4</t>
+  </si>
+  <si>
+    <t>IMPUTATION 4: plausible value</t>
+  </si>
+  <si>
+    <t>pv_5</t>
+  </si>
+  <si>
+    <t>IMPUTATION 5: plausible value</t>
+  </si>
+  <si>
+    <t>pvkat_pooled</t>
+  </si>
+  <si>
+    <t>categorical plausible value</t>
+  </si>
+  <si>
+    <t>pvkat_1</t>
+  </si>
+  <si>
+    <t>IMPUTATION 1: Kompetenzstufe des plausible value</t>
+  </si>
+  <si>
+    <t>pvkat_2</t>
+  </si>
+  <si>
+    <t>IMPUTATION 2: Kompetenzstufe des plausible value</t>
+  </si>
+  <si>
+    <t>pvkat_3</t>
+  </si>
+  <si>
+    <t>IMPUTATION 3: Kompetenzstufe des plausible value</t>
+  </si>
+  <si>
+    <t>pvkat_4</t>
+  </si>
+  <si>
+    <t>IMPUTATION 4: Kompetenzstufe des plausible value</t>
+  </si>
+  <si>
+    <t>pvkat_5</t>
+  </si>
+  <si>
+    <t>This is an example.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -256,9 +266,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -540,14 +559,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -613,14 +634,12 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2"/>
       <c r="F2" t="s">
         <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2"/>
       <c r="I2" t="s">
         <v>22</v>
       </c>
@@ -649,7 +668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -662,14 +681,12 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3"/>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3"/>
       <c r="I3" t="s">
         <v>25</v>
       </c>
@@ -698,7 +715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -720,7 +737,6 @@
       <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="H4"/>
       <c r="I4" t="s">
         <v>27</v>
       </c>
@@ -749,7 +765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -771,7 +787,6 @@
       <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="H5"/>
       <c r="I5" t="s">
         <v>29</v>
       </c>
@@ -800,7 +815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -822,7 +837,6 @@
       <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="H6"/>
       <c r="I6" t="s">
         <v>32</v>
       </c>
@@ -851,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -873,7 +887,6 @@
       <c r="G7" t="s">
         <v>37</v>
       </c>
-      <c r="H7"/>
       <c r="I7" t="s">
         <v>20</v>
       </c>
@@ -902,7 +915,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -924,7 +937,6 @@
       <c r="G8" t="s">
         <v>37</v>
       </c>
-      <c r="H8"/>
       <c r="I8" t="s">
         <v>20</v>
       </c>
@@ -953,7 +965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -975,7 +987,6 @@
       <c r="G9" t="s">
         <v>37</v>
       </c>
-      <c r="H9"/>
       <c r="I9" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1026,7 +1037,6 @@
       <c r="G10" t="s">
         <v>37</v>
       </c>
-      <c r="H10"/>
       <c r="I10" t="s">
         <v>41</v>
       </c>
@@ -1055,7 +1065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1068,14 +1078,12 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11"/>
       <c r="F11" t="s">
         <v>20</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
       </c>
-      <c r="H11"/>
       <c r="I11" t="s">
         <v>46</v>
       </c>
@@ -1104,7 +1112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1126,7 +1134,6 @@
       <c r="G12" t="s">
         <v>45</v>
       </c>
-      <c r="H12"/>
       <c r="I12" t="s">
         <v>20</v>
       </c>
@@ -1155,7 +1162,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1177,7 +1184,6 @@
       <c r="G13" t="s">
         <v>45</v>
       </c>
-      <c r="H13"/>
       <c r="I13" t="s">
         <v>20</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1228,7 +1234,6 @@
       <c r="G14" t="s">
         <v>45</v>
       </c>
-      <c r="H14"/>
       <c r="I14" t="s">
         <v>20</v>
       </c>
@@ -1257,7 +1262,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1279,7 +1284,6 @@
       <c r="G15" t="s">
         <v>45</v>
       </c>
-      <c r="H15"/>
       <c r="I15" t="s">
         <v>20</v>
       </c>
@@ -1308,7 +1312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1330,7 +1334,6 @@
       <c r="G16" t="s">
         <v>45</v>
       </c>
-      <c r="H16"/>
       <c r="I16" t="s">
         <v>20</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1372,14 +1375,12 @@
       <c r="D17" t="s">
         <v>20</v>
       </c>
-      <c r="E17"/>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="G17" t="s">
         <v>45</v>
       </c>
-      <c r="H17"/>
       <c r="I17" t="s">
         <v>58</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -1430,7 +1431,6 @@
       <c r="G18" t="s">
         <v>45</v>
       </c>
-      <c r="H18"/>
       <c r="I18" t="s">
         <v>20</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1481,7 +1481,6 @@
       <c r="G19" t="s">
         <v>45</v>
       </c>
-      <c r="H19"/>
       <c r="I19" t="s">
         <v>20</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1532,7 +1531,6 @@
       <c r="G20" t="s">
         <v>45</v>
       </c>
-      <c r="H20"/>
       <c r="I20" t="s">
         <v>20</v>
       </c>
@@ -1561,7 +1559,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1583,7 +1581,6 @@
       <c r="G21" t="s">
         <v>45</v>
       </c>
-      <c r="H21"/>
       <c r="I21" t="s">
         <v>20</v>
       </c>
@@ -1612,7 +1609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1634,7 +1631,6 @@
       <c r="G22" t="s">
         <v>45</v>
       </c>
-      <c r="H22"/>
       <c r="I22" t="s">
         <v>20</v>
       </c>
@@ -1665,6 +1661,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>